<commit_message>
updated tooltips in config
</commit_message>
<xml_diff>
--- a/input/config.xlsx
+++ b/input/config.xlsx
@@ -474,7 +474,7 @@
     <t xml:space="preserve">KOMMENT: config.xlsx előző verziójából másolva, mind2 évre ugyanaz!</t>
   </si>
   <si>
-    <t xml:space="preserve">FB</t>
+    <t xml:space="preserve">FH1</t>
   </si>
   <si>
     <t xml:space="preserve">Alaptevékenység finanszírozási egyenlege</t>
@@ -483,7 +483,7 @@
     <t xml:space="preserve">A finanszírozási pénzmozgások irányát mutatja, a külső finanszírozásból származó bevételeket (pl. hitelfelvétel) és az adósságszolgálatot (pl. tőketörlesztést) szembeállítva. Bizonyos befektetési tranzakciók is itt kerülnek kimutatásra. A pozitív egyenleg nettó eladósodást jelent, amiből kiadások finanszírozhatók, a negatív érték nettó hiteltörlesztést mutat.</t>
   </si>
   <si>
-    <t xml:space="preserve">RE</t>
+    <t xml:space="preserve">FH2</t>
   </si>
   <si>
     <t xml:space="preserve">Alaptevékenység szabad maradványa</t>
@@ -2713,16 +2713,16 @@
   <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="109.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="109.69"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2736,7 +2736,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -2747,7 +2747,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -2780,7 +2780,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>31</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>35</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
         <v>38</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
         <v>40</v>
       </c>
@@ -2912,7 +2912,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
         <v>43</v>
       </c>
@@ -2923,7 +2923,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
         <v>45</v>
       </c>
@@ -2934,7 +2934,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
         <v>48</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
         <v>51</v>
       </c>
@@ -2956,7 +2956,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
         <v>54</v>
       </c>
@@ -2967,7 +2967,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
         <v>57</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
         <v>60</v>
       </c>
@@ -2989,7 +2989,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
         <v>63</v>
       </c>
@@ -3000,7 +3000,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
         <v>66</v>
       </c>
@@ -3011,7 +3011,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
         <v>69</v>
       </c>
@@ -3022,7 +3022,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
         <v>71</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
         <v>74</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
         <v>77</v>
       </c>
@@ -3055,7 +3055,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="302.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
         <v>80</v>
       </c>
@@ -3066,7 +3066,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
         <v>83</v>
       </c>
@@ -3077,7 +3077,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
         <v>86</v>
       </c>
@@ -3088,7 +3088,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
         <v>89</v>
       </c>
@@ -3099,7 +3099,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
         <v>92</v>
       </c>
@@ -3110,7 +3110,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
         <v>95</v>
       </c>
@@ -3121,7 +3121,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="254.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
         <v>97</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
         <v>100</v>
       </c>
@@ -3154,7 +3154,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
         <v>106</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
         <v>109</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
         <v>112</v>
       </c>
@@ -3187,7 +3187,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
         <v>115</v>
       </c>
@@ -3198,7 +3198,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
         <v>117</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
         <v>119</v>
       </c>
@@ -3220,7 +3220,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
         <v>122</v>
       </c>
@@ -3231,7 +3231,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
         <v>125</v>
       </c>
@@ -3242,7 +3242,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
         <v>128</v>
       </c>
@@ -3253,7 +3253,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
         <v>131</v>
       </c>
@@ -3264,7 +3264,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
         <v>133</v>
       </c>
@@ -3275,7 +3275,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
         <v>136</v>
       </c>
@@ -3286,7 +3286,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
         <v>139</v>
       </c>
@@ -3297,7 +3297,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
         <v>142</v>
       </c>
@@ -3324,19 +3324,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C242"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="109.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="109.69"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5958,6 +5958,8 @@
         <v>802</v>
       </c>
     </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -5974,7 +5976,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C242"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5982,11 +5984,11 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="109.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="109.69"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8608,6 +8610,8 @@
         <v>802</v>
       </c>
     </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -8632,7 +8636,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.48"/>

</xml_diff>

<commit_message>
removed signo, swapped FTx nodes
</commit_message>
<xml_diff>
--- a/input/config.xlsx
+++ b/input/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" state="visible" r:id="rId2"/>
@@ -1027,13 +1027,13 @@
     <t xml:space="preserve">Államháztartáson belüli megelőlegezések</t>
   </si>
   <si>
+    <t xml:space="preserve">FT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fejlesztési hitel, értékpapírok eladása</t>
+  </si>
+  <si>
     <t xml:space="preserve">FT1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fejlesztési hitel, értékpapírok eladása</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FT2</t>
   </si>
   <si>
     <t xml:space="preserve">Áthúzódó projektek, szabad maradvány, elszámolások</t>
@@ -2810,13 +2810,13 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.85"/>
@@ -3408,12 +3408,12 @@
   <dimension ref="A1:C317"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A90" activeCellId="0" sqref="A90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.86"/>
@@ -6385,13 +6385,13 @@
   </sheetPr>
   <dimension ref="A1:C314"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A92" activeCellId="0" sqref="A92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.86"/>
@@ -9342,7 +9342,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.43"/>

</xml_diff>

<commit_message>
fixed milestone img path in config
</commit_message>
<xml_diff>
--- a/input/config.xlsx
+++ b/input/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1588" uniqueCount="871">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1588" uniqueCount="870">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -2638,7 +2638,7 @@
 A MÁTRA MŰVELŐDÉSI KÖZPONT (MMK) energetikai korszerűsítése és a „Kulcs Projekt” című pályázatok egymásra építve, együttesen teszik lehetővé az intézmény teljeskörű modernizálását. Az energetikai korszerűsítés keretében megvalósult az épület falainak és tetejének hőszigetelése, a külső nyílászárók cseréje, valamint az épület színháztermének szellőzési lehetősége és klimatizálása is. A színházterem fölötti lapostetőn napelemeket helyeztek el. A fejlesztésnek köszönhetően az MMK a környezeti terhelés csökkentésével, innovatív megoldások beépítésével modern közösségi térként fogadja látogatóit. A ‘KULCS PROJEKT’ keretében az épület belső közösségi funkciójának, infrastruktúrájának és eszközállományának megújítása a cél. Felújításra kerül az elektromos hálózat, emellett a mai elvárásoknak megfelelő tűz-, és érintésvédelmi fejlesztések történnek. A fejlesztések révén az épület funkciói bővülnek, így hatékonyabban tudja majd kiszolgálni a helyi közösség igényeit.</t>
   </si>
   <si>
-    <t xml:space="preserve">Jeruzsálem úti óvoda.jpg</t>
+    <t xml:space="preserve">assets/img/jeruzsalem-uti-ovoda.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">A Jeruzsálem úti bölcsőde és óvoda fejlesztése</t>
@@ -2647,9 +2647,6 @@
     <t xml:space="preserve">Kódszám: TOP-1.4.1-16-HE1-2017-00021
 Támogatási összeg: 249 999 080 Ft.
 A fejlesztési koncepció az volt, hogy a bölcsődei új férőhelyek létrehozásán túlmenően az óvoda és bölcsőde meglévő épületegyüttese energetikailag is megfeleljen a mai kor igényeinek. A projekt lezárultával a gondozási egységek száma egyről kettőre, a gyerekszobák száma kettőről négyre emelkedik, ennek köszönhetően a fogadható gyermekek létszáma 26 főről 50 főre nőhet. A megvalósítás során megtörténik az intézmény energetikai célú felújítása, szigeteléssel, nyílászáró cserével, továbbá a bölcsőde részére új épületrész épül.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assets/img/jeruzsalem-uti-ovoda.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">assets/img/korona.jpg</t>
@@ -3019,13 +3016,13 @@
   </sheetPr>
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="1" sqref="C8 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.85"/>
@@ -3639,10 +3636,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A315" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C319" activeCellId="0" sqref="C319"/>
+      <selection pane="bottomLeft" activeCell="C319" activeCellId="1" sqref="C8 C319"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.86"/>
@@ -6643,10 +6640,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C95" activeCellId="0" sqref="C95"/>
+      <selection pane="bottomLeft" activeCell="C95" activeCellId="1" sqref="C8 C95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.86"/>
@@ -9639,13 +9636,13 @@
   </sheetPr>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="118.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="118.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.43"/>
@@ -9807,7 +9804,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
@@ -9823,14 +9820,14 @@
         <v>2020</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
+        <v>865</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>866</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>867</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="118.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9839,14 +9836,14 @@
         <v>13</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
+        <v>865</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>866</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>867</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="118.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9855,14 +9852,14 @@
         <v>2020</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
+        <v>868</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>869</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>870</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="118.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9871,14 +9868,14 @@
         <v>13</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
+        <v>868</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>869</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>870</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added background colors into inex text
</commit_message>
<xml_diff>
--- a/input/config.xlsx
+++ b/input/config.xlsx
@@ -370,9 +370,7 @@
     <t xml:space="preserve">inex.text</t>
   </si>
   <si>
-    <t xml:space="preserve">**Segítünk értelmezni!** Az oldalon Gyöngyös Önkormányzatának és intézményeinek 2020-as költségvetése látható. A mérleg a költségvetési rendeletben szereplő főösszeget mutatja be. Ahhoz, hogy megértsük, miből gazdálkodik ténylegesen a város, érdemes elkülöníteni a saját intézmények finanszírozását (**irányítószervi támogatás**), ami számviteli okból duplán szerepel a főösszegben, illetve az éven belüli **folyószámlahitel-ügyleteket**. Ezek nélkül Gyöngyös költségvetési kiadásai meghaladták a 11,5 milliárd Ft-ot. Ebből látta el a város szerteágazó feladatait.
-A bevételek és kiadások is felbonthatók működési és felhalmozási tételekre. A **működési költségvetés** a zavartalan feladatellátást biztosítja, míg a **felhalmozási költségvetés** beruházásokhoz, felújításokhoz kapcsolódik, melyek célja tartós eszközök beszerzése, a tevékenység bővítése, modernizálása. A működési bevételek (törvényben meghatározott állami normatívák, helyi adók, a nyújtott szolgáltatások ellenértéke) és kiadások (bérek, rezsiköltségek, nyújtott támogatások) rendszeresen, ciklikusan jelentkeznek. Ezzel szemben a felhalmozási tételek eseti jellegűek, gyakran több éves költségvetési hatással (pl. uniós és állami pályázatok).
-A működési költségvetés többlete mellett az önkormányzat fenntartható, színvonalas feladatellátásához szükséges fejlesztésekre fordíthatók a kifejezetten felhalmozásra kapott bevételek és a **finanszírozási költségvetés** többlete. Utóbbi csekély részt fejlesztési hiteleket jelent, amit a város jövőbeni működési többletéből tud visszafizetni. Gyöngyös finanszírozási bevételeinek nagyja az előző évi gazdálkodás maradványa: a folyamatban lévő uniós fejlesztések még fel nem használt támogatásai, illetve a megelőző évről maradt szabad maradvány. Mindezek egyelőre tervszámok, a ténylegesen teljesült összegeket a 2021-ben elfogadandó zárszámadás tartalmazza. Ennek birtokában az oldalon a költségvetés kormányzati funkciók szerinti bontását is elérhetővé tesszük.</t>
+    <t xml:space="preserve">**Segítünk értelmezni!** Az oldalon Gyöngyös Önkormányzatának és intézményeinek 2020-as költségvetése látható. A mérleg a költségvetési rendeletben szereplő főösszeget mutatja be. Ahhoz, hogy megértsük, miből gazdálkodik ténylegesen a város, érdemes elkülöníteni a saját intézmények finanszírozását (**&lt;span style="background: #d7d7d7"&gt;irányítószervi támogatás&lt;/span&gt;**), ami számviteli okból duplán szerepel a főösszegben, illetve az éven belüli **&lt;span style="background: #d7d7d7"&gt;folyószámlahitel-ügyleteket&lt;/span&gt;**. Ezek nélkül Gyöngyös költségvetési kiadásai meghaladták a 11,5 milliárd Ft-ot. Ebből látta el a város szerteágazó feladatait.  A bevételek és kiadások is felbonthatók működési és felhalmozási tételekre. A **&lt;span style="background: #a3b1c8"&gt;működési költségvetés&lt;/span&gt;** a zavartalan feladatellátást biztosítja, míg a **&lt;span style="background: #c1a3c8"&gt;felhalmozási költségvetés&lt;/span&gt;** beruházásokhoz, felújításokhoz kapcsolódik, melyek célja tartós eszközök beszerzése, a tevékenység bővítése, modernizálása. A működési bevételek (törvényben meghatározott állami normatívák, helyi adók, a nyújtott szolgáltatások ellenértéke) és kiadások (bérek, rezsiköltségek, nyújtott támogatások) rendszeresen, ciklikusan jelentkeznek. Ezzel szemben a felhalmozási tételek eseti jellegűek, gyakran több éves költségvetési hatással (pl. uniós és állami pályázatok).  A működési költségvetés többlete mellett az önkormányzat fenntartható, színvonalas feladatellátásához szükséges fejlesztésekre fordíthatók a kifejezetten felhalmozásra kapott bevételek és a **&lt;span style="background: #ace3c4"&gt;finanszírozási költségvetés&lt;/span&gt;** többlete. Utóbbi csekély részt fejlesztési hiteleket jelent, amit a város jövőbeni működési többletéből tud visszafizetni. Gyöngyös finanszírozási bevételeinek nagyja az előző évi gazdálkodás maradványa: a folyamatban lévő uniós fejlesztések még fel nem használt támogatásai, illetve a megelőző évről maradt szabad maradvány. Mindezek egyelőre tervszámok, a ténylegesen teljesült összegeket a 2021-ben elfogadandó zárszámadás tartalmazza. Ennek birtokában az oldalon a költségvetés kormányzati funkciók szerinti bontását is elérhetővé tesszük.</t>
   </si>
   <si>
     <t xml:space="preserve">Mérleg szakasz ábra alatti szövege. Markdown jelölések használhatóak (pl. formázás, linkek).</t>
@@ -3150,12 +3148,12 @@
   <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.85"/>
@@ -3591,7 +3589,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="611.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
         <v>107</v>
       </c>
@@ -3769,7 +3767,7 @@
       <selection pane="bottomLeft" activeCell="C143" activeCellId="0" sqref="C143"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.86"/>
@@ -6790,7 +6788,7 @@
       <selection pane="bottomLeft" activeCell="C319" activeCellId="0" sqref="C319"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.86"/>
@@ -9806,7 +9804,7 @@
       <selection pane="bottomLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.43"/>

</xml_diff>

<commit_message>
added bgcolors to inex text
</commit_message>
<xml_diff>
--- a/input/config.xlsx
+++ b/input/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" state="visible" r:id="rId2"/>
@@ -347,7 +347,7 @@
     <t xml:space="preserve">inex.text</t>
   </si>
   <si>
-    <t xml:space="preserve">**Segítünk értelmezni!** Az ábra Mintaváros önkormányzatának és intézményeinek éves költségvetését mutatja mérlegszerű bontásban. A bevételek és kiadások is felbonthatók működési és felhalmozási tételekre. A működési költségvetés a zavartalan feladatellátást biztosítja, míg a felhalmozási költségvetés beruházásokhoz, felújításokhoz kapcsolódik, melyek célja tartós eszközök beszerzése, a tevékenység bővítése, modernizálása. A működési bevételek (törvényben meghatározott állami normatívák, helyi adók, a nyújtott szolgáltatások ellenértéke) és kiadások (bérek, rezsiköltségek, nyújtott támogatások) rendszeresen, ciklikusan jelentkeznek. Ezzel szemben a felhalmozási tételek eseti jellegűek, gyakran több éves költségvetési hatással (pl. uniós és állami pályázatok). A finanszírozási többlet java része az előző évi gazdálkodás maradványa: a folyamatban lévő fejlesztések még fel nem használt támogatásai, illetve az előző évről maradt szabad maradvány. </t>
+    <t xml:space="preserve">**Segítünk értelmezni!** Az ábra Mintaváros önkormányzatának és intézményeinek éves költségvetését mutatja mérlegszerű bontásban. A bevételek és kiadások is felbonthatók működési és felhalmozási tételekre. A &lt;span style="background: #a3b1c8"&gt;működési költségvetés&lt;/span&gt; a zavartalan feladatellátást biztosítja, míg a &lt;span style="background: #c1a3c8"&gt;felhalmozási költségvetés&lt;/span&gt; beruházásokhoz, felújításokhoz kapcsolódik, melyek célja tartós eszközök beszerzése, a tevékenység bővítése, modernizálása. A működési bevételek (törvényben meghatározott állami normatívák, helyi adók, a nyújtott szolgáltatások ellenértéke) és kiadások (bérek, rezsiköltségek, nyújtott támogatások) rendszeresen, ciklikusan jelentkeznek. Ezzel szemben a felhalmozási tételek eseti jellegűek, gyakran több éves költségvetési hatással (pl. uniós és állami pályázatok). A &lt;span style="background: #ace3c4"&gt;finanszírozási többlet&lt;/span&gt; java része az előző évi gazdálkodás maradványa: a folyamatban lévő fejlesztések még fel nem használt támogatásai, illetve az előző évről maradt szabad maradvány.</t>
   </si>
   <si>
     <t xml:space="preserve">Mérleg szakasz ábra alatti szövege. Markdown jelölések használhatóak (pl. formázás, linkek).</t>
@@ -3102,13 +3102,13 @@
   </sheetPr>
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.23046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.22265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.13"/>
@@ -4667,10 +4667,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A301" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A307" activeCellId="0" sqref="A307"/>
+      <selection pane="bottomLeft" activeCell="A307" activeCellId="1" sqref="B40 A307"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.23046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.22265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.5"/>
@@ -8560,10 +8560,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A98" activeCellId="0" sqref="A98"/>
+      <selection pane="bottomLeft" activeCell="A98" activeCellId="1" sqref="B40 A98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.23046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.22265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.87"/>
@@ -12556,13 +12556,13 @@
   </sheetPr>
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="1" sqref="B40 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.23046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.22265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.61"/>

</xml_diff>

<commit_message>
added new line + &nbsp;s into inex text
</commit_message>
<xml_diff>
--- a/input/config.xlsx
+++ b/input/config.xlsx
@@ -347,7 +347,8 @@
     <t xml:space="preserve">inex.text</t>
   </si>
   <si>
-    <t xml:space="preserve">**Segítünk értelmezni!** Az ábra Mintaváros önkormányzatának és intézményeinek éves költségvetését mutatja mérlegszerű bontásban. A bevételek és kiadások is felbonthatók működési és felhalmozási tételekre. A &lt;span style="background: #a3b1c8"&gt;működési költségvetés&lt;/span&gt; a zavartalan feladatellátást biztosítja, míg a &lt;span style="background: #c1a3c8"&gt;felhalmozási költségvetés&lt;/span&gt; beruházásokhoz, felújításokhoz kapcsolódik, melyek célja tartós eszközök beszerzése, a tevékenység bővítése, modernizálása. A működési bevételek (törvényben meghatározott állami normatívák, helyi adók, a nyújtott szolgáltatások ellenértéke) és kiadások (bérek, rezsiköltségek, nyújtott támogatások) rendszeresen, ciklikusan jelentkeznek. Ezzel szemben a felhalmozási tételek eseti jellegűek, gyakran több éves költségvetési hatással (pl. uniós és állami pályázatok). A &lt;span style="background: #ace3c4"&gt;finanszírozási többlet&lt;/span&gt; java része az előző évi gazdálkodás maradványa: a folyamatban lévő fejlesztések még fel nem használt támogatásai, illetve az előző évről maradt szabad maradvány.</t>
+    <t xml:space="preserve">**Segítünk értelmezni!** Az ábra Mintaváros önkormányzatának és intézményeinek éves költségvetését mutatja mérlegszerű bontásban.
+A bevételek és kiadások is felbonthatók működési és felhalmozási tételekre. A &lt;span style="background: #a3b1c8"&gt;működési&amp;nbsp;költségvetés&lt;/span&gt; a zavartalan feladatellátást biztosítja, míg a &lt;span style="background: #c1a3c8"&gt;felhalmozási&amp;nbsp;költségvetés&lt;/span&gt; beruházásokhoz, felújításokhoz kapcsolódik, melyek célja tartós eszközök beszerzése, a tevékenység bővítése, modernizálása. A működési bevételek (törvényben meghatározott állami normatívák, helyi adók, a nyújtott szolgáltatások ellenértéke) és kiadások (bérek, rezsiköltségek, nyújtott támogatások) rendszeresen, ciklikusan jelentkeznek. Ezzel szemben a felhalmozási tételek eseti jellegűek, gyakran több éves költségvetési hatással (pl. uniós és állami pályázatok). A &lt;span style="background: #ace3c4"&gt;finanszírozási&amp;nbsp;többlet&lt;/span&gt; java része az előző évi gazdálkodás maradványa: a folyamatban lévő fejlesztések még fel nem használt támogatásai, illetve az előző évről maradt szabad maradvány.</t>
   </si>
   <si>
     <t xml:space="preserve">Mérleg szakasz ábra alatti szövege. Markdown jelölések használhatóak (pl. formázás, linkek).</t>
@@ -2960,7 +2961,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -3105,10 +3106,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
+      <selection pane="bottomLeft" activeCell="B41" activeCellId="0" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.22265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.21484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.13"/>
@@ -4667,10 +4668,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A301" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A307" activeCellId="1" sqref="B40 A307"/>
+      <selection pane="bottomLeft" activeCell="A307" activeCellId="0" sqref="A307"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.22265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.21484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.5"/>
@@ -8560,10 +8561,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A98" activeCellId="1" sqref="B40 A98"/>
+      <selection pane="bottomLeft" activeCell="A98" activeCellId="0" sqref="A98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.22265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.21484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.87"/>
@@ -12559,10 +12560,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="1" sqref="B40 A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.22265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.21484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.61"/>

</xml_diff>

<commit_message>
moved 1st pic to cover
</commit_message>
<xml_diff>
--- a/input/config.xlsx
+++ b/input/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1712" uniqueCount="913">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1710" uniqueCount="912">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -2707,9 +2707,6 @@
   </si>
   <si>
     <t xml:space="preserve">descriptionInMarkdown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/assets/img/1.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">/assets/vid/1.mp4</t>
@@ -3103,7 +3100,7 @@
   </sheetPr>
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B41" activeCellId="0" sqref="B41"/>
@@ -12557,10 +12554,10 @@
   </sheetPr>
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12600,17 +12597,15 @@
       <c r="B2" s="3" t="n">
         <v>2020</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
         <v>894</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>895</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="10" t="s">
         <v>896</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>897</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12620,17 +12615,15 @@
       <c r="B3" s="3" t="n">
         <v>2021</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="s">
         <v>894</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>895</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="10" t="s">
         <v>896</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>897</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12641,14 +12634,14 @@
         <v>2020</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="3" t="s">
+        <v>898</v>
+      </c>
+      <c r="F4" s="22" t="s">
         <v>899</v>
-      </c>
-      <c r="F4" s="22" t="s">
-        <v>900</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12659,14 +12652,14 @@
         <v>2021</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="3" t="s">
+        <v>898</v>
+      </c>
+      <c r="F5" s="22" t="s">
         <v>899</v>
-      </c>
-      <c r="F5" s="22" t="s">
-        <v>900</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12677,14 +12670,14 @@
         <v>2020</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="3" t="s">
+        <v>901</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>902</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>903</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12695,14 +12688,14 @@
         <v>2021</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="3" t="s">
+        <v>901</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>902</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>903</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12713,14 +12706,14 @@
         <v>2020</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="12" t="s">
+        <v>904</v>
+      </c>
+      <c r="F8" s="22" t="s">
         <v>905</v>
-      </c>
-      <c r="F8" s="22" t="s">
-        <v>906</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12731,14 +12724,14 @@
         <v>2021</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="12" t="s">
+        <v>904</v>
+      </c>
+      <c r="F9" s="22" t="s">
         <v>905</v>
-      </c>
-      <c r="F9" s="22" t="s">
-        <v>906</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12749,14 +12742,14 @@
         <v>2020</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="3" t="s">
+        <v>907</v>
+      </c>
+      <c r="F10" s="12" t="s">
         <v>908</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>909</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12767,14 +12760,14 @@
         <v>2021</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="3" t="s">
+        <v>907</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>908</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>909</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12783,14 +12776,14 @@
         <v>2020</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="23" t="s">
+        <v>910</v>
+      </c>
+      <c r="F12" s="24" t="s">
         <v>911</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12799,14 +12792,14 @@
         <v>2021</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="23" t="s">
+        <v>910</v>
+      </c>
+      <c r="F13" s="24" t="s">
         <v>911</v>
-      </c>
-      <c r="F13" s="24" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
added new config and milestone pics
</commit_message>
<xml_diff>
--- a/input/config.xlsx
+++ b/input/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="709">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -258,7 +258,7 @@
     <t xml:space="preserve">welcome.title</t>
   </si>
   <si>
-    <t xml:space="preserve">TISZTELT KECSEKMÉTI POLGÁROK!</t>
+    <t xml:space="preserve">TISZTELT KECSKEMÉTI POLGÁROK!</t>
   </si>
   <si>
     <t xml:space="preserve">Köszöntő szakasz címsora.</t>
@@ -2099,6 +2099,40 @@
   </si>
   <si>
     <t xml:space="preserve">descriptionInMarkdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/assets/img/1elv.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amit a kormány elvon, arra nagy szükség van Kecskeméten, mutat rá a polgármester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A kecskeméti polgármester a helyi vállalkozások és vállalkozói érdekképviseletek képviselőivel tárgyalt a gazdasági kihívásokról és a 2021. évi városi költségvetésről. Szemereyné Pataki Klaudia úgy foglalt állást, hogy „A vállalkozások látják, hogy épül a város, ezért többen is úgy döntöttek, hogy teljes egészében befizetik az iparűzési adót, és nem élnek az általuk igényelhető kedvezménnyel.”
+A Fidesz-kormány már 2019 ősze előtt – amikor még szinte minden önkormányzat élén kormánypárti politikus ült – megpróbálkozott azzal, hogy az önkormányzatok legfőbb bevételét jelentő iparűzési adó egyrészét elvonja, ha úgy tetszik, átrendezi. Ezt akkor a Fideszen belüli ellenlobbi akadályozta meg. 
+A 2019 őszi politikai változásokat követően, miután az ország felét és a fővárost elvesztette a Fidesz, újra napirendre került az önkormányzatiság vitája, ami azóta tovább fokozódott a településeket érintő forráselvonások és adónövelés következtében. Az Orbán-kormány a gazdasági válságra hivatkozva ugyanis elvonta a gépjármű adót, megnövelte a szolidaritási adót, és az ingyenes parkolás bevezetésével súlyos milliókat vett ki a városok zsebéből.
+Tovább a [teljes cikkre]. (https://kecsup.hu/2021/01/amit-a-kormany-elvon-arra-nagy-szukseg-van-kecskemeten-mutat-ra-a-polgarmester/)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/assets/img/2onk.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Az önkormányzatiság közös értékünk és nem megszüntetendő politikai termék</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A kormányzati kommunikáció szerint, ami forráselvonásként jelenik meg az önkormányzatoknál, az nem más mint: válságkezelés és gazdaságélénkítés. A kormány a válságkezelésre hivatkozva elvonta a városok bevételeinek jelentős részét, amit utakra, közvilágításra, szociális ellátásra, helyi közlekedésre fordíthatnának. Az iparűzési adó csökkentése azért nem nyújt érdemi segítséget a bajba jutott vállalkozásoknak, mert egy nagyon alacsony adónemről van szó. Egy kecskeméti vállalkozás adóköltségének ez mindössze 1,8%-a. Egyesek szerint ez a korbács és mézesmadzag politikája, nem a szabadság és a felelősség politikája.
+Az, hogy milyen a várospolitika és mennyire élhető a városunk nagyban függ attól, hogy meddig nyújtózkodhat az önkormányzat. A koronavírus-járványban az Orbán-kormány nem csak forráselvonásokkal sújtja az önkormányzatokat, de teljesen kihagyja őket a járványkezelésből is. A legtöbben a partnerség- és az információhiányra panaszkodnak.
+Tovább a [teljes cikkre]. ( https://kecsup.hu/2020/12/megszorito-csomagot-kuldott-orban-viktor-kecskemetnek/)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/assets/img/3kozl.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kecskemét közlekedése – forró téma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Évtizedes probléma a Belváros tehermentesítése, amit a döntéshozók többsége ugyan elismer és a városi stratégiai dokumentumok is beszélnek róla, de átfogó, szisztematikus cselekvés még sem történt a gyalogos, a kerékpáros és a buszos közlekedés előnybe hozásáért az elmúlt 10 évben. Ami viszont változott az a 110 ezres lakosú Kecskeméten regisztrált gépjárművek száma, amely 2010 óta folyamatosan emelkedik és a számuk ma már több mint 61 ezer.
+Hogy a politikai akarat, vagy a forrás hiányzik-e, vagy mindkettő, netalántán a tudatos várostervezés, arról megoszlanak a vélemények. Egy-egy képviselő által tett szándéknyilatkozattól és civil javaslattól eltekintve a Belváros közlekedésének egésze komolyan nem került még a kecskemétiek elé. 
+Tovább a [teljes cikkre]. (https://kecsup.hu/2021/03/belvarosi-kozlekedes-nevlegesen-zero-emisszios-zona-a-valosagban-zsakuta-1-resz/)</t>
   </si>
   <si>
     <t xml:space="preserve">/assets/vid/1.mp4</t>
@@ -2258,7 +2292,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2295,7 +2329,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2382,13 +2432,13 @@
   </sheetPr>
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="66" zoomScaleNormal="66" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="66" zoomScaleNormal="66" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.9921875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40"/>
@@ -2406,7 +2456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>3</v>
       </c>
@@ -2505,7 +2555,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>25</v>
       </c>
@@ -2965,7 +3015,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>141</v>
       </c>
@@ -2979,7 +3029,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="http://kecskemet.koko.deepdata.hu/"/>
-    <hyperlink ref="B11" r:id="rId2" display="http://kecskemet.koko.deepdata.hu/assets"/>
+    <hyperlink ref="B11" r:id="rId2" display="http://kecskemet.koko.deepdata.hu/assets/img/mintavaros-01.png"/>
     <hyperlink ref="B53" r:id="rId3" display="https://forms.gle/MCxioUo6LB97me6b9 "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3000,12 +3050,12 @@
   <dimension ref="A1:C262"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C260" activeCellId="0" sqref="C260"/>
+      <selection pane="bottomLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.9921875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50"/>
@@ -5436,15 +5486,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.9921875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5"/>
@@ -5472,52 +5522,100 @@
         <v>690</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2"/>
-      <c r="B2" s="9" t="n">
+    <row r="2" s="13" customFormat="true" ht="252" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9"/>
+      <c r="B2" s="10" t="n">
         <v>2021</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="11" t="s">
         <v>691</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="D2" s="9"/>
+      <c r="E2" s="11" t="s">
         <v>692</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="12" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2"/>
-      <c r="B3" s="9" t="n">
+    <row r="3" s="13" customFormat="true" ht="220.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9"/>
+      <c r="B3" s="10" t="n">
         <v>2021</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="11" t="s">
         <v>694</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="9" t="s">
+      <c r="D3" s="9"/>
+      <c r="E3" s="11" t="s">
         <v>695</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="12" t="s">
         <v>696</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2"/>
-      <c r="B4" s="9" t="n">
+    <row r="4" s="13" customFormat="true" ht="173.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10" t="n">
         <v>2021</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="11" t="s">
         <v>697</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
+      <c r="D4" s="9"/>
+      <c r="E4" s="11" t="s">
         <v>698</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="12" t="s">
         <v>699</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2"/>
+      <c r="B5" s="10" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>701</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2"/>
+      <c r="B6" s="10" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="10" t="s">
+        <v>704</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2"/>
+      <c r="B7" s="10" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>706</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>708</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified URLs in config
</commit_message>
<xml_diff>
--- a/input/config.xlsx
+++ b/input/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" state="visible" r:id="rId2"/>
@@ -36,7 +36,7 @@
     <t xml:space="preserve">url</t>
   </si>
   <si>
-    <t xml:space="preserve">http://kecskemet.koko.deepdata.hu/</t>
+    <t xml:space="preserve">http://kecskemetkoltsegvetese.kecsup.hu</t>
   </si>
   <si>
     <t xml:space="preserve">A weboldal leendő URL-je. Keresőoptimalizálásnál és megosztásnál van szerepe.</t>
@@ -102,7 +102,7 @@
     <t xml:space="preserve">seo.ogImage</t>
   </si>
   <si>
-    <t xml:space="preserve">http://kecskemet.koko.deepdata.hu/assets/img/mintavaros-01.png</t>
+    <t xml:space="preserve">http://kecskemetkoltsegvetese.kecsup.hu/assets/img/cover.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Facebook/Twitter megosztáskor az előnézeti kártyában megjelenő kép URL-je.</t>
@@ -2107,37 +2107,10 @@
     <t xml:space="preserve">Amit a kormány elvon, arra nagy szükség van Kecskeméten, mutat rá a polgármester</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve">A kecskeméti polgármester a helyi vállalkozások és vállalkozói érdekképviseletek képviselőivel tárgyalt a gazdasági kihívásokról és a 2021. évi városi költségvetésről. Szemereyné Pataki Klaudia úgy foglalt állást, hogy „A vállalkozások látják, hogy épül a város, ezért többen is úgy döntöttek, hogy teljes egészében befizetik az iparűzési adót, és nem élnek az általuk igényelhető kedvezménnyel.”
+    <t xml:space="preserve">A kecskeméti polgármester a helyi vállalkozások és vállalkozói érdekképviseletek képviselőivel tárgyalt a gazdasági kihívásokról és a 2021. évi városi költségvetésről. Szemereyné Pataki Klaudia úgy foglalt állást, hogy „A vállalkozások látják, hogy épül a város, ezért többen is úgy döntöttek, hogy teljes egészében befizetik az iparűzési adót, és nem élnek az általuk igényelhető kedvezménnyel.”
 A Fidesz-kormány már 2019 ősze előtt – amikor még szinte minden önkormányzat élén kormánypárti politikus ült – megpróbálkozott azzal, hogy az önkormányzatok legfőbb bevételét jelentő iparűzési adó egyrészét elvonja, ha úgy tetszik, átrendezi. Ezt akkor a Fideszen belüli ellenlobbi akadályozta meg. 
 A 2019 őszi politikai változásokat követően, miután az ország felét és a fővárost elvesztette a Fidesz, újra napirendre került az önkormányzatiság vitája, ami azóta tovább fokozódott a településeket érintő forráselvonások és adónövelés következtében. Az Orbán-kormány a gazdasági válságra hivatkozva ugyanis elvonta a gépjármű adót, megnövelte a szolidaritási adót, és az ingyenes parkolás bevezetésével súlyos milliókat vett ki a városok zsebéből.
-Tovább a [teljes cikkre](</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve">https://kecsup.hu/2021/01/amit-a-kormany-elvon-arra-nagy-szukseg-van-kecskemeten-mutat-ra-a-polgarmester/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
+Tovább a [teljes cikkre](https://kecsup.hu/2021/01/amit-a-kormany-elvon-arra-nagy-szukseg-van-kecskemeten-mutat-ra-a-polgarmester/)</t>
   </si>
   <si>
     <t xml:space="preserve">/assets/img/2onk.jpg</t>
@@ -2146,36 +2119,9 @@
     <t xml:space="preserve">Az önkormányzatiság közös értékünk és nem megszüntetendő politikai termék</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve">A kormányzati kommunikáció szerint, ami forráselvonásként jelenik meg az önkormányzatoknál, az nem más mint: válságkezelés és gazdaságélénkítés. A kormány a válságkezelésre hivatkozva elvonta a városok bevételeinek jelentős részét, amit utakra, közvilágításra, szociális ellátásra, helyi közlekedésre fordíthatnának. Az iparűzési adó csökkentése azért nem nyújt érdemi segítséget a bajba jutott vállalkozásoknak, mert egy nagyon alacsony adónemről van szó. Egy kecskeméti vállalkozás adóköltségének ez mindössze 1,8%-a. Egyesek szerint ez a korbács és mézesmadzag politikája, nem a szabadság és a felelősség politikája.
+    <t xml:space="preserve">A kormányzati kommunikáció szerint, ami forráselvonásként jelenik meg az önkormányzatoknál, az nem más mint: válságkezelés és gazdaságélénkítés. A kormány a válságkezelésre hivatkozva elvonta a városok bevételeinek jelentős részét, amit utakra, közvilágításra, szociális ellátásra, helyi közlekedésre fordíthatnának. Az iparűzési adó csökkentése azért nem nyújt érdemi segítséget a bajba jutott vállalkozásoknak, mert egy nagyon alacsony adónemről van szó. Egy kecskeméti vállalkozás adóköltségének ez mindössze 1,8%-a. Egyesek szerint ez a korbács és mézesmadzag politikája, nem a szabadság és a felelősség politikája.
 Az, hogy milyen a várospolitika és mennyire élhető a városunk nagyban függ attól, hogy meddig nyújtózkodhat az önkormányzat. A koronavírus-járványban az Orbán-kormány nem csak forráselvonásokkal sújtja az önkormányzatokat, de teljesen kihagyja őket a járványkezelésből is. A legtöbben a partnerség- és az információhiányra panaszkodnak.
-Tovább a [teljes cikkre]( </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve">https://kecsup.hu/2020/12/megszorito-csomagot-kuldott-orban-viktor-kecskemetnek/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
+Tovább a [teljes cikkre]( https://kecsup.hu/2020/12/megszorito-csomagot-kuldott-orban-viktor-kecskemetnek/)</t>
   </si>
   <si>
     <t xml:space="preserve">/assets/img/3kozl.jpg</t>
@@ -2353,7 +2299,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2396,6 +2342,10 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -2485,13 +2435,13 @@
   </sheetPr>
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="66" zoomScaleNormal="66" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="66" zoomScaleNormal="66" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
+      <selection pane="bottomLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.96875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40"/>
@@ -2509,7 +2459,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>3</v>
       </c>
@@ -2608,7 +2558,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>25</v>
       </c>
@@ -3081,9 +3031,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://kecskemet.koko.deepdata.hu/"/>
-    <hyperlink ref="B11" r:id="rId2" display="http://kecskemet.koko.deepdata.hu/assets/img/mintavaros-01.png"/>
-    <hyperlink ref="B53" r:id="rId3" display="https://forms.gle/MCxioUo6LB97me6b9 "/>
+    <hyperlink ref="B2" r:id="rId1" display="http://kecskemetkoltsegvetese.kecsup.hu"/>
+    <hyperlink ref="B53" r:id="rId2" display="https://forms.gle/MCxioUo6LB97me6b9 "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3108,7 +3057,7 @@
       <selection pane="bottomLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.96875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50"/>
@@ -5541,13 +5490,13 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.96875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5"/>
@@ -5619,7 +5568,7 @@
       <c r="E4" s="8" t="s">
         <v>698</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="12" t="s">
         <v>699</v>
       </c>
     </row>
@@ -5632,10 +5581,10 @@
       <c r="D5" s="2" t="s">
         <v>700</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="13" t="s">
         <v>701</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="13" t="s">
         <v>702</v>
       </c>
     </row>
@@ -5651,7 +5600,7 @@
       <c r="E6" s="10" t="s">
         <v>704</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="13" t="s">
         <v>705</v>
       </c>
     </row>
@@ -5673,8 +5622,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="https://kecsup.hu/2021/01/amit-a-kormany-elvon-arra-nagy-szukseg-van-kecskemeten-mutat-ra-a-polgarmester/"/>
-    <hyperlink ref="F3" r:id="rId2" display="https://kecsup.hu/2020/12/megszorito-csomagot-kuldott-orban-viktor-kecskemetnek/"/>
+    <hyperlink ref="F2" r:id="rId1" display="A kecskeméti polgármester a helyi vállalkozások és vállalkozói érdekképviseletek képviselőivel tárgyalt a gazdasági kihívásokról és a 2021. évi városi költségvetésről. Szemereyné Pataki Klaudia úgy foglalt állást, hogy „A vállalkozások látják, hogy épül a város, ezért többen is úgy döntöttek, hogy teljes egészében befizetik az iparűzési adót, és nem élnek az általuk igényelhető kedvezménnyel.”&#10;A Fidesz-kormány már 2019 ősze előtt – amikor még szinte minden önkormányzat élén kormánypárti politikus ült – megpróbálkozott azzal, hogy az önkormányzatok legfőbb bevételét jelentő iparűzési adó egyrészét elvonja, ha úgy tetszik, átrendezi. Ezt akkor a Fideszen belüli ellenlobbi akadályozta meg. &#10;A 2019 őszi politikai változásokat követően, miután az ország felét és a fővárost elvesztette a Fidesz, újra napirendre került az önkormányzatiság vitája, ami azóta tovább fokozódott a településeket érintő forráselvonások és adónövelés következtében. Az Orbán-kormány a gazdasági válságra hivatkozva ugyanis elvonta a gépjármű adót, megnövelte a szolidaritási adót, és az ingyenes parkolás bevezetésével súlyos milliókat vett ki a városok zsebéből.&#10;Tovább a [teljes cikkre](https://kecsup.hu/2021/01/amit-a-kormany-elvon-arra-nagy-szukseg-van-kecskemeten-mutat-ra-a-polgarmester/)"/>
+    <hyperlink ref="F3" r:id="rId2" display="A kormányzati kommunikáció szerint, ami forráselvonásként jelenik meg az önkormányzatoknál, az nem más mint: válságkezelés és gazdaságélénkítés. A kormány a válságkezelésre hivatkozva elvonta a városok bevételeinek jelentős részét, amit utakra, közvilágításra, szociális ellátásra, helyi közlekedésre fordíthatnának. Az iparűzési adó csökkentése azért nem nyújt érdemi segítséget a bajba jutott vállalkozásoknak, mert egy nagyon alacsony adónemről van szó. Egy kecskeméti vállalkozás adóköltségének ez mindössze 1,8%-a. Egyesek szerint ez a korbács és mézesmadzag politikája, nem a szabadság és a felelősség politikája.&#10;Az, hogy milyen a várospolitika és mennyire élhető a városunk nagyban függ attól, hogy meddig nyújtózkodhat az önkormányzat. A koronavírus-járványban az Orbán-kormány nem csak forráselvonásokkal sújtja az önkormányzatokat, de teljesen kihagyja őket a járványkezelésből is. A legtöbben a partnerség- és az információhiányra panaszkodnak.&#10;Tovább a [teljes cikkre]( https://kecsup.hu/2020/12/megszorito-csomagot-kuldott-orban-viktor-kecskemetnek/)"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
moved milestone pics+vids into separate dir
</commit_message>
<xml_diff>
--- a/input/config.xlsx
+++ b/input/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" state="visible" r:id="rId2"/>
@@ -2709,7 +2709,7 @@
     <t xml:space="preserve">descriptionInMarkdown</t>
   </si>
   <si>
-    <t xml:space="preserve">/assets/vid/1.mp4</t>
+    <t xml:space="preserve">1.mp4</t>
   </si>
   <si>
     <t xml:space="preserve">Közérthető költségvetés - Mi ez?</t>
@@ -2718,7 +2718,7 @@
     <t xml:space="preserve">A fenti videóra kattintva játékos formában is megnézheted, miért tartottuk fontosnak, hogy a helyi közpénzek átlátható bemutatását segítő eszközt fejlesszünk. Ha érdekel, kik vagyunk, nézz körül a [K-Monitor honlapján!](http://k-monitor.hu)</t>
   </si>
   <si>
-    <t xml:space="preserve">/assets/img/2.jpg</t>
+    <t xml:space="preserve">2.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Részvételi költségvetés</t>
@@ -2728,7 +2728,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">/assets/img/3.jpg</t>
+    <t xml:space="preserve">3.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Költségvetési ABC</t>
@@ -2737,7 +2737,7 @@
     <t xml:space="preserve">A **Költségvetési ABC - Hallasd a hangod a helyi pénzügyekben** című kiadvány civileknek és állampolgároknak készült. Arról szól, hogyan születik és mit tartalmaz egy önkormányzat költségvetése és hogyan szólhatsz bele a településed gazdálkodásába. A kiadványban kérdés-válasz formában, közérhetőségre törekedve tekintjük át az önkormányzatok működését, gazdálkodását, a költségvetési folyamatot, a mindenhol elérhető dokumentumok alapvető összefüggéseit és az átláthatóság, részvétel főbb technikáit.  Kiadványunk [innen tölthető le](https://k-monitor.hu/cikkek/20190604-koltsegvetesi-abc-hallasd-a-hangod-a-helyi-penzugyekben).</t>
   </si>
   <si>
-    <t xml:space="preserve">/assets/img/4.jpg</t>
+    <t xml:space="preserve">4.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">A koronavírus-járvány pénzügyi hatásai</t>
@@ -2751,7 +2751,7 @@
 A járványhelyzet kezelése érdekében Mintaváros önkormányzata számos lépést tett, melyek egy része pénzügyi kiadással járt. Ilyen volt a maszkok és fertőtlenítőszerek beszerzése, tesztek vásárlása és ovónők tesztelésének lebonyolítása. Emellett rendkívüli veszélyhelyzeti támogatást is bevezetett a rászorulók részére. </t>
   </si>
   <si>
-    <t xml:space="preserve">/assets/img/5.jpg</t>
+    <t xml:space="preserve">5.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Mintaváros főterének felújítása</t>
@@ -2760,7 +2760,7 @@
     <t xml:space="preserve">Mintaváros pályázatos támogatásból a város főterének megújítását tervezi. A főtér megújítása során a zöldfelületek aránya 20%-al nő, a térre új utcabútorok kerülnek, valamint a tér melletti utca sétálóutcává alakul át. A tér északi szegletében található önkormányzati tulajdonú helység infoponttá alakul, a déli részén pedig közWC kerül kialakításra. A projekt időtartama 1,5 év, a munkálatok várhatóan 2021 végére fejeződnek be. </t>
   </si>
   <si>
-    <t xml:space="preserve">/assets/img/6.jpg</t>
+    <t xml:space="preserve">6.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Hogyan lehet nálunk is közérthető a költségvetés?</t>
@@ -3100,13 +3100,13 @@
   </sheetPr>
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B53" activeCellId="0" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.20703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.13"/>
@@ -4668,7 +4668,7 @@
       <selection pane="bottomLeft" activeCell="A307" activeCellId="0" sqref="A307"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.20703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.5"/>
@@ -8561,7 +8561,7 @@
       <selection pane="bottomLeft" activeCell="A98" activeCellId="0" sqref="A98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.20703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.87"/>
@@ -12554,13 +12554,13 @@
   </sheetPr>
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.20703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.61"/>

</xml_diff>

<commit_message>
renamed "Fejlesztések" to "Magyarázatok"
</commit_message>
<xml_diff>
--- a/input/config.xlsx
+++ b/input/config.xlsx
@@ -133,7 +133,7 @@
     <t xml:space="preserve">navBar.milestones</t>
   </si>
   <si>
-    <t xml:space="preserve">Fejlesztések</t>
+    <t xml:space="preserve">Magyarázatok</t>
   </si>
   <si>
     <t xml:space="preserve">Fejlesztések szakaszra mutató link szövege a felső navigációs sávban.</t>
@@ -3071,12 +3071,12 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="bottomLeft" activeCell="B45" activeCellId="0" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.13"/>
@@ -4598,7 +4598,7 @@
       <selection pane="bottomLeft" activeCell="A307" activeCellId="0" sqref="A307"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.5"/>
@@ -8491,7 +8491,7 @@
       <selection pane="bottomLeft" activeCell="A98" activeCellId="0" sqref="A98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.87"/>
@@ -12490,7 +12490,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.61"/>

</xml_diff>